<commit_message>
refactor(Book): update book excel template
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/book-template.xlsx
+++ b/src/main/resources/templates/book-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project_fromC\backend\library\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E46BB7-4F0D-4FCD-B908-76E4657BB7E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5850BCA-E36C-4C55-84BB-D01DAB957532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    jx:area(lastCell=”I5”)</t>
+    jx:area(lastCell=”K5”)</t>
       </text>
     </comment>
     <comment ref="A5" authorId="1" shapeId="0" xr:uid="{358541DD-91E1-449B-9FE4-15224C314FEC}">
@@ -44,7 +44,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    jx:each(items=”books” var=”book” lastCell=”I5”)</t>
+    jx:each(items=”books” var=”book” lastCell=”K5”)</t>
       </text>
     </comment>
   </commentList>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Created at</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Updated By</t>
   </si>
   <si>
-    <t>${book.code}</t>
-  </si>
-  <si>
     <t>${book.title}</t>
   </si>
   <si>
@@ -115,6 +112,21 @@
   </si>
   <si>
     <t>${createdAt}</t>
+  </si>
+  <si>
+    <t>${book.id}</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>${book.language}</t>
+  </si>
+  <si>
+    <t>${book.description}</t>
   </si>
 </sst>
 </file>
@@ -464,10 +476,10 @@
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A1" dT="2025-03-12T11:56:35.47" personId="{01880B02-8677-478F-A89D-4EA850D706CB}" id="{BC4AC809-338B-4A88-B68D-2C25BBC522CB}">
-    <text>jx:area(lastCell=”I5”)</text>
+    <text>jx:area(lastCell=”K5”)</text>
   </threadedComment>
   <threadedComment ref="A5" dT="2025-03-12T11:58:29.59" personId="{01880B02-8677-478F-A89D-4EA850D706CB}" id="{358541DD-91E1-449B-9FE4-15224C314FEC}">
-    <text>jx:each(items=”books” var=”book” lastCell=”I5”)</text>
+    <text>jx:each(items=”books” var=”book” lastCell=”K5”)</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -477,7 +489,7 @@
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,6 +503,8 @@
     <col min="7" max="7" width="38.42578125" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
     <col min="9" max="9" width="30.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -498,7 +512,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -553,8 +567,12 @@
       <c r="I4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="J4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -567,31 +585,37 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>